<commit_message>
Store, Integer Reg-Reg additions
</commit_message>
<xml_diff>
--- a/RISC-V_decode.xlsx
+++ b/RISC-V_decode.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
   <si>
     <t>RV32I</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Fence</t>
   </si>
   <si>
-    <t>Arithmentic Immediate</t>
-  </si>
-  <si>
     <t>AUIPC</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>Atomic</t>
   </si>
   <si>
-    <t>Arithmetic Register</t>
-  </si>
-  <si>
     <t>decimal</t>
   </si>
   <si>
@@ -104,21 +98,6 @@
     <t>31 -  funct7  - 25</t>
   </si>
   <si>
-    <t>24 -  Rs2 - 20</t>
-  </si>
-  <si>
-    <t>19 - Rs1 - 15</t>
-  </si>
-  <si>
-    <t>11 -  Rd  - 7</t>
-  </si>
-  <si>
-    <t>6 - opcode - 0</t>
-  </si>
-  <si>
-    <t>11 - imm[4:0] - 7</t>
-  </si>
-  <si>
     <t>31 -  imm[11:5]  - 25</t>
   </si>
   <si>
@@ -161,9 +140,6 @@
     <t>RV32i Instruction types</t>
   </si>
   <si>
-    <t>ArithReg</t>
-  </si>
-  <si>
     <t>SYS</t>
   </si>
   <si>
@@ -176,12 +152,6 @@
     <t>60</t>
   </si>
   <si>
-    <t>0017b793</t>
-  </si>
-  <si>
-    <t>Arithmetic Immediate</t>
-  </si>
-  <si>
     <t>Integer Multiply</t>
   </si>
   <si>
@@ -189,13 +159,55 @@
   </si>
   <si>
     <t>Integer Remainder</t>
+  </si>
+  <si>
+    <t>0237b767</t>
+  </si>
+  <si>
+    <t>fef42423</t>
+  </si>
+  <si>
+    <t>0200006f</t>
+  </si>
+  <si>
+    <t>fec42703</t>
+  </si>
+  <si>
+    <t>0ff7f793</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Integer Reg-Reg</t>
+  </si>
+  <si>
+    <t>Integer Reg-Imm</t>
+  </si>
+  <si>
+    <t>24 -          Rs2         - 20</t>
+  </si>
+  <si>
+    <t>19 -         Rs1         - 15</t>
+  </si>
+  <si>
+    <t>11 -     imm[4:0]     - 7</t>
+  </si>
+  <si>
+    <t>11 -           Rd           - 7</t>
+  </si>
+  <si>
+    <t>6 -        opcode        - 0</t>
+  </si>
+  <si>
+    <t>007F4533</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,8 +251,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -315,8 +334,37 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -415,15 +463,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -447,9 +574,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -460,66 +584,282 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="5" builtinId="10"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="42">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF53D2FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -561,6 +901,44 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF53D2FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -712,61 +1090,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -794,6 +1122,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCC00"/>
+      <color rgb="FF53D2FF"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FFFFEB9C"/>
     </mruColors>
@@ -1099,7 +1429,7 @@
   <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,6 +1439,7 @@
     <col min="8" max="9" width="9.140625" customWidth="1"/>
     <col min="11" max="12" width="9.140625" customWidth="1"/>
     <col min="16" max="16" width="9.5703125" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" customWidth="1"/>
     <col min="21" max="22" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1117,17 +1448,26 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="T2" t="s">
         <v>51</v>
       </c>
+      <c r="U2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17"/>
+      <c r="X2" s="20"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -1138,13 +1478,29 @@
       <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="T3" t="s">
+        <v>49</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="V3" s="22"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="20" t="str">
+        <f>IF(C28,   IF(J15=0,"LB",(IF(J15=1,"LH",(IF(J15=2,"LW",IF(J15=4,"LBU",IF(J15=5,"LHU"," "))))))), " ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y3" t="str">
+        <f>IF(C28, CONCATENATE("X",K15,", 0x",DEC2HEX(D15),"(X",H15,")"), " ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C4" t="b">
-        <f>OR(C28,D28,E28,H28,I28,J28,L28,M28,N28,O28,P28,Q28)</f>
+        <f>OR(C28,D28,E28,G28,H28,I28,K28,L28,M28,N28,O28,P28)</f>
         <v>1</v>
       </c>
       <c r="D4" t="b">
@@ -1155,16 +1511,41 @@
         <f>NOT(OR(C4,D4))</f>
         <v>0</v>
       </c>
+      <c r="U4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="V4" s="26"/>
+      <c r="W4" s="27"/>
+      <c r="X4" s="20" t="str">
+        <f>IF(D28, "Fence", "")</f>
+        <v/>
+      </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>5</v>
+      </c>
+      <c r="T5" t="s">
+        <v>50</v>
+      </c>
+      <c r="U5" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="V5" s="22"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="20" t="str">
+        <f>IF(E28,IF(K15,IF(J15=0,"ADDI",IF(J15=1,"SLLI",IF(J15=2,"SLTI",IF(J15=3,"SLTIU",IF(J15=4,"XORI",IF(AND(J15=5,D12=0),"SRLI",IF(AND(J15=5,D12=32),"SRAI",IF(J15=6,"ORI",IF(J15=7,"ANDI"," ")))))))))), " ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y5" t="str">
+        <f>IF(E28, CONCATENATE("X",K15,", X",H15,", 0x",D15), " ")</f>
+        <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>HEX2DEC(A2)</f>
-        <v>1554323</v>
+        <v>4277412899</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>8</v>
@@ -1175,31 +1556,48 @@
       <c r="O6" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="U6" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="V6" s="26"/>
+      <c r="W6" s="27"/>
+      <c r="X6" s="20"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>42</v>
+      <c r="A7" s="16" t="s">
+        <v>35</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="M7" s="4" t="str">
         <f>DEC2BIN(M8)</f>
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="N7" s="4" t="str">
         <f>DEC2BIN(N8)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O7" s="4" t="str">
         <f>DEC2BIN(O8)</f>
         <v>11</v>
       </c>
-      <c r="U7" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="V7" s="34"/>
-      <c r="W7" s="34"/>
+      <c r="T7" t="s">
+        <v>47</v>
+      </c>
+      <c r="U7" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="V7" s="59"/>
+      <c r="W7" s="60"/>
+      <c r="X7" s="45" t="str">
+        <f>IF(H28, IF(J18=0,"SB",IF(J18=1,"SH",IF(J18=2,"SW"," ")))," ")</f>
+        <v>SW</v>
+      </c>
+      <c r="Y7" t="str">
+        <f>IF(H28,CONCATENATE("X",F18,", 0x",DEC2HEX(_xlfn.BITLSHIFT(D18,5)+K18),"(X",H18,")")," ")</f>
+        <v>X15, 0xFE8(X8)</v>
+      </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1207,131 +1605,143 @@
         <v>96</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M8">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,2),31)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N8">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,2),7)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <f>_xlfn.BITAND(A6,3)</f>
         <v>3</v>
       </c>
-      <c r="U8" s="26" t="s">
-        <v>9</v>
+      <c r="U8" s="25" t="s">
+        <v>13</v>
       </c>
       <c r="V8" s="26"/>
-      <c r="W8" s="26"/>
-      <c r="X8" t="str">
-        <f>IF(C28,    IF(J15=0,"LB",(IF(J15=1,"LH",(IF(J15=2,"LW",IF(J15=4,"LBU",IF(J15=5,"LHU"," "))))))), " ")</f>
+      <c r="W8" s="27"/>
+      <c r="X8" s="20"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="T9" t="s">
+        <v>59</v>
+      </c>
+      <c r="U9" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="V9" s="53"/>
+      <c r="W9" s="54"/>
+      <c r="X9" s="45" t="str">
+        <f>IF(J28, IF(D12=0,IF(J12=0,"ADD",IF(J12=1, "SLL",IF(J12=2,"SLT",IF(J12=3,"SLTU",IF(J12=4,"XOR",IF(J12=5,"SRL",IF(J12=6,"OR",IF(J12=7,"AND", " ")))))))), IF(D12=BIN2DEC(100000), IF(J12=0,"SUB",IF(J12=1,"SRA", " ")))), " ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y8" t="str">
-        <f>IF(C28, CONCATENATE("X",K15,", 0x",DEC2HEX(D15),"(X",H15,")"), " ")</f>
+      <c r="Y9" t="str">
+        <f>IF(J28, CONCATENATE("R",K12,", R",H12," ,R",F12), " ")</f>
         <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="U9" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="V9" s="26"/>
-      <c r="W9" s="26"/>
-      <c r="X9" t="str">
-        <f>IF(D28, "Fence", "")</f>
-        <v/>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="U10" s="26" t="s">
-        <v>52</v>
+        <v>29</v>
+      </c>
+      <c r="U10" s="25" t="s">
+        <v>43</v>
       </c>
       <c r="V10" s="26"/>
-      <c r="W10" s="26"/>
-      <c r="X10" t="str">
-        <f>IF(E28,  IF(K15,IF(J15=0,"ADDI",IF(J15=1,"SLLI",IF(J15=2,"SLTI",IF(J15=3,"SLTIU",IF(J15=4,"XORI",IF(AND(J15=5,D12=0),"SRLI",IF(AND(J15=5,D12=32),"SRAI",IF(J15=6,"ORI",IF(J15=7,"ANDI"," ")))))))))),"")</f>
-        <v>SLTIU</v>
-      </c>
-      <c r="Y10" t="str">
-        <f>IF(E28, CONCATENATE("X",K15,", X",H15,", 0x",D15), " ")</f>
-        <v>X15, X15, 0x1</v>
-      </c>
+      <c r="W10" s="27"/>
+      <c r="X10" s="20"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="D11" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="23"/>
-      <c r="H11" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="25"/>
+      <c r="D11" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="37"/>
+      <c r="F11" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="33"/>
+      <c r="H11" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="34"/>
       <c r="J11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" s="27"/>
-      <c r="M11" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="N11" s="24"/>
-      <c r="U11" s="26" t="s">
-        <v>12</v>
+      <c r="K11" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="L11" s="38"/>
+      <c r="M11" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="N11" s="55"/>
+      <c r="O11" s="56" t="str">
+        <f>IF(J28," &lt;---- Integer Register Register format"," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="P11" s="56"/>
+      <c r="Q11" s="56"/>
+      <c r="R11" s="56"/>
+      <c r="U11" s="25" t="s">
+        <v>44</v>
       </c>
       <c r="V11" s="26"/>
-      <c r="W11" s="26"/>
+      <c r="W11" s="27"/>
+      <c r="X11" s="20"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="19">
+        <v>20</v>
+      </c>
+      <c r="D12" s="29">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,25),127)</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="19">
+        <v>127</v>
+      </c>
+      <c r="E12" s="30"/>
+      <c r="F12" s="29">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,20),15)</f>
-        <v>1</v>
-      </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="19">
-        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,15),15)</f>
         <v>15</v>
       </c>
-      <c r="I12" s="21"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="29">
+        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,15),31)</f>
+        <v>8</v>
+      </c>
+      <c r="I12" s="30"/>
       <c r="J12" s="7">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,12),7)</f>
-        <v>3</v>
-      </c>
-      <c r="K12" s="19">
-        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,7),15)</f>
-        <v>15</v>
-      </c>
-      <c r="L12" s="21"/>
-      <c r="M12" s="19" t="str">
+        <v>2</v>
+      </c>
+      <c r="K12" s="29">
+        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,7),31)</f>
+        <v>8</v>
+      </c>
+      <c r="L12" s="30"/>
+      <c r="M12" s="29" t="str">
         <f>CONCATENATE("0x",DEC2HEX(_xlfn.BITAND(A6,127)))</f>
-        <v>0x13</v>
-      </c>
-      <c r="N12" s="21"/>
-      <c r="U12" s="26" t="s">
-        <v>13</v>
+        <v>0x23</v>
+      </c>
+      <c r="N12" s="30"/>
+      <c r="P12" s="6" t="str">
+        <f>IF(J28, X9, " ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Q12" s="24" t="str">
+        <f>Y9</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
+      <c r="U12" s="25" t="s">
+        <v>45</v>
       </c>
       <c r="V12" s="26"/>
-      <c r="W12" s="26"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="20"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D13" s="8"/>
@@ -1345,468 +1755,475 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
-      <c r="U13" s="26" t="s">
-        <v>14</v>
+      <c r="U13" s="25" t="s">
+        <v>15</v>
       </c>
       <c r="V13" s="26"/>
-      <c r="W13" s="26"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="20"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="D14" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="25"/>
+      <c r="D14" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="34"/>
       <c r="J14" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K14" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="L14" s="11"/>
-      <c r="M14" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="N14" s="24"/>
-      <c r="O14" t="str">
-        <f>IF(C28,"  &lt;---- Load Instruction format", IF(E28,"  &lt;---- Arithmetic Immediate format"," "))</f>
-        <v xml:space="preserve">  &lt;---- Arithmetic Immediate format</v>
-      </c>
-      <c r="U14" s="26" t="s">
-        <v>46</v>
+      <c r="K14" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="L14" s="51"/>
+      <c r="M14" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="N14" s="44"/>
+      <c r="O14" s="24" t="str">
+        <f>IF(C28,"  &lt;---- Load Instruction format", IF(E28,"  &lt;---- Arithmetic Immediate format",  IF(N28,"  &lt;---- JALR format"," ")))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="U14" s="25" t="s">
+        <v>16</v>
       </c>
       <c r="V14" s="26"/>
-      <c r="W14" s="26"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="20"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="19">
+        <v>21</v>
+      </c>
+      <c r="D15" s="29">
         <f>(_xlfn.BITAND(_xlfn.BITRSHIFT(A6,20),4095))</f>
-        <v>1</v>
-      </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="19">
-        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,15),15)</f>
-        <v>15</v>
-      </c>
-      <c r="I15" s="21"/>
+        <v>4079</v>
+      </c>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="29">
+        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,15),31)</f>
+        <v>8</v>
+      </c>
+      <c r="I15" s="30"/>
       <c r="J15" s="7">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,12),7)</f>
-        <v>3</v>
-      </c>
-      <c r="K15" s="19">
-        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,7),15)</f>
-        <v>15</v>
-      </c>
-      <c r="L15" s="21"/>
-      <c r="M15" s="19" t="str">
+        <v>2</v>
+      </c>
+      <c r="K15" s="29">
+        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,7),31)</f>
+        <v>8</v>
+      </c>
+      <c r="L15" s="30"/>
+      <c r="M15" s="29" t="str">
         <f>CONCATENATE("0x",DEC2HEX(_xlfn.BITAND(A6,127)))</f>
-        <v>0x13</v>
-      </c>
-      <c r="N15" s="21"/>
+        <v>0x23</v>
+      </c>
+      <c r="N15" s="30"/>
       <c r="P15" s="6" t="str">
-        <f>IF(C28,   X8,  X10 )</f>
-        <v>SLTIU</v>
-      </c>
-      <c r="Q15" s="26" t="str">
-        <f>IF(C28,  Y8,    IF(E28, Y10, " "))</f>
-        <v>X15, X15, 0x1</v>
-      </c>
-      <c r="R15" s="26"/>
-      <c r="S15" s="26"/>
-      <c r="U15" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="V15" s="26"/>
-      <c r="W15" s="26"/>
+        <f>IF(C28, X3, IF(E28,X5,IF(N28,X15," ")))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Q15" s="24" t="str">
+        <f>IF(C28, Y3, IF(E28, Y5,IF(N28,Y15," ")))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
+      <c r="T15" t="s">
+        <v>46</v>
+      </c>
+      <c r="U15" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="V15" s="40"/>
+      <c r="W15" s="40"/>
+      <c r="X15" s="20" t="str">
+        <f>IF(N28,  "JALR", " ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y15" t="str">
+        <f>IF(N28,CONCATENATE("R",K15,", 0x",DEC2HEX(D15),"(R",H15,")"),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
-      <c r="U16" s="26" t="s">
+      <c r="T16" t="s">
+        <v>48</v>
+      </c>
+      <c r="U16" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="V16" s="41"/>
+      <c r="W16" s="41"/>
+      <c r="X16" s="20" t="str">
+        <f>IF(O28,  "JAL", " ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y16" t="str">
+        <f>IF(O28, CONCATENATE("X",K24,", 0x", DEC2HEX(_xlfn.BITLSHIFT(E24,1)+_xlfn.BITLSHIFT(G24,11)+_xlfn.BITLSHIFT(H24,12)+_xlfn.BITLSHIFT(IF(D24, 4095,0),20)+A8)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="D17" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="35"/>
+      <c r="F17" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="V16" s="26"/>
-      <c r="W16" s="26"/>
-    </row>
-    <row r="17" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="D17" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="23"/>
-      <c r="H17" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="25"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="I17" s="34"/>
       <c r="J17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K17" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="L17" s="28"/>
-      <c r="M17" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="N17" s="24"/>
-      <c r="O17" t="str">
-        <f>IF(I28,"  &lt;---- Store Instruction format",IF(O28,"JALR format"," "))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="U17" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="V17" s="26"/>
-      <c r="W17" s="26"/>
-    </row>
-    <row r="18" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="K17" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="L17" s="39"/>
+      <c r="M17" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="N17" s="57"/>
+      <c r="O17" s="61" t="str">
+        <f>IF(H28,"  &lt;---- Store Instruction format"," ")</f>
+        <v xml:space="preserve">  &lt;---- Store Instruction format</v>
+      </c>
+      <c r="P17" s="61"/>
+      <c r="Q17" s="61"/>
+      <c r="R17" s="61"/>
+      <c r="U17" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="V17" s="42"/>
+      <c r="W17" s="42"/>
+      <c r="X17" s="20"/>
+    </row>
+    <row r="18" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="19">
+        <v>22</v>
+      </c>
+      <c r="D18" s="29">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,25),127)</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="19">
+        <v>127</v>
+      </c>
+      <c r="E18" s="30"/>
+      <c r="F18" s="29">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,20),15)</f>
-        <v>1</v>
-      </c>
-      <c r="G18" s="21"/>
-      <c r="H18" s="19">
-        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,15),15)</f>
         <v>15</v>
       </c>
-      <c r="I18" s="21"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="29">
+        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,15),31)</f>
+        <v>8</v>
+      </c>
+      <c r="I18" s="30"/>
       <c r="J18" s="7">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,12),7)</f>
-        <v>3</v>
-      </c>
-      <c r="K18" s="19">
+        <v>2</v>
+      </c>
+      <c r="K18" s="29">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,7),15)</f>
-        <v>15</v>
-      </c>
-      <c r="L18" s="21"/>
-      <c r="M18" s="19" t="str">
+        <v>8</v>
+      </c>
+      <c r="L18" s="30"/>
+      <c r="M18" s="29" t="str">
         <f>CONCATENATE("0x",DEC2HEX(_xlfn.BITAND(A6,127)))</f>
-        <v>0x13</v>
-      </c>
-      <c r="N18" s="21"/>
-      <c r="U18" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="V18" s="26"/>
-      <c r="W18" s="26"/>
-    </row>
-    <row r="19" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="U19" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="V19" s="26"/>
-      <c r="W19" s="26"/>
-    </row>
-    <row r="20" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="D20" s="18" t="s">
+        <v>0x23</v>
+      </c>
+      <c r="N18" s="30"/>
+      <c r="P18" s="6" t="str">
+        <f>X7</f>
+        <v>SW</v>
+      </c>
+      <c r="Q18" s="24" t="str">
+        <f>Y7</f>
+        <v>X15, 0xFE8(X8)</v>
+      </c>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="U18" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="V18" s="42"/>
+      <c r="W18" s="42"/>
+      <c r="X18" s="20"/>
+    </row>
+    <row r="19" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="U19" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="V19" s="42"/>
+      <c r="W19" s="42"/>
+      <c r="X19" s="20"/>
+    </row>
+    <row r="20" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="D20" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="L20" s="38"/>
+      <c r="M20" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="N20" s="28"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+    </row>
+    <row r="21" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="29">
+        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,12),1048575)</f>
+        <v>1044290</v>
+      </c>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="29">
+        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,7),31)</f>
+        <v>8</v>
+      </c>
+      <c r="L21" s="30"/>
+      <c r="M21" s="29" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(_xlfn.BITAND(A6,127)))</f>
+        <v>0x23</v>
+      </c>
+      <c r="N21" s="30"/>
+    </row>
+    <row r="23" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="D23" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="L20" s="27"/>
-      <c r="M20" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="N20" s="24"/>
-      <c r="U20" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="V20" s="26"/>
-      <c r="W20" s="26"/>
-      <c r="X20" t="str">
-        <f>IF(O28,  "JALR", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="19">
-        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,12),1048575)</f>
-        <v>379</v>
-      </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="19">
-        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,7),15)</f>
-        <v>15</v>
-      </c>
-      <c r="L21" s="21"/>
-      <c r="M21" s="19" t="str">
-        <f>CONCATENATE("0x",DEC2HEX(_xlfn.BITAND(A6,127)))</f>
-        <v>0x13</v>
-      </c>
-      <c r="N21" s="21"/>
-      <c r="U21" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="V21" s="26"/>
-      <c r="W21" s="26"/>
-      <c r="X21" t="str">
-        <f>IF(P28,  "JAL", "")</f>
-        <v/>
-      </c>
-      <c r="Y21" t="str">
-        <f>IF(P28, CONCATENATE("R",K24,", 0x", DEC2HEX(_xlfn.BITLSHIFT(E24,1)+_xlfn.BITLSHIFT(G24,11)+_xlfn.BITLSHIFT(H24,12)+_xlfn.BITLSHIFT(IF(D24, 4095,0),20)+A8)), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="U22" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="V22" s="26"/>
-      <c r="W22" s="26"/>
-    </row>
-    <row r="23" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="H23" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="L23" s="27"/>
-      <c r="M23" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="N23" s="24"/>
-      <c r="O23" t="str">
-        <f>IF(P28,"  &lt;---- JAL format"," ")</f>
+      <c r="E23" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="31"/>
+      <c r="G23" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="L23" s="38"/>
+      <c r="M23" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="N23" s="43"/>
+      <c r="O23" s="24" t="str">
+        <f>IF(O28,"  &lt;---- JAL format"," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U23" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="V23" s="26"/>
-      <c r="W23" s="26"/>
-    </row>
-    <row r="24" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="D24" s="16">
+      <c r="P23" s="24"/>
+      <c r="Q23" s="24"/>
+      <c r="R23" s="24"/>
+    </row>
+    <row r="24" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="15">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,31),1)</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="19">
+        <v>1</v>
+      </c>
+      <c r="E24" s="29">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,21),1023)</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="16">
+        <v>1015</v>
+      </c>
+      <c r="F24" s="30"/>
+      <c r="G24" s="15">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,20),1)</f>
         <v>1</v>
       </c>
-      <c r="H24" s="19">
+      <c r="H24" s="29">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,12),255)</f>
-        <v>123</v>
-      </c>
-      <c r="I24" s="20"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="19">
-        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,7),15)</f>
+        <v>66</v>
+      </c>
+      <c r="I24" s="32"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="29">
+        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,7),31)</f>
+        <v>8</v>
+      </c>
+      <c r="L24" s="30"/>
+      <c r="M24" s="29" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(_xlfn.BITAND(A6,127)))</f>
+        <v>0x23</v>
+      </c>
+      <c r="N24" s="30"/>
+      <c r="P24" s="6" t="str">
+        <f>X16</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Q24" s="24" t="str">
+        <f>Y16</f>
+        <v/>
+      </c>
+      <c r="R24" s="24"/>
+      <c r="S24" s="24"/>
+      <c r="T24" s="24" t="str">
+        <f>IF(O28, CONCATENATE("PC+4 = 0x", DEC2HEX(A8+4)," ",IF(K24=0,"NOT ", ""),"written to X",K24), "")</f>
+        <v/>
+      </c>
+      <c r="U24" s="24"/>
+      <c r="V24" s="24"/>
+    </row>
+    <row r="26" spans="3:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="3:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="46"/>
+      <c r="G27" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J27" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="K27" s="50"/>
+      <c r="L27" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L24" s="21"/>
-      <c r="M24" s="19" t="str">
-        <f>CONCATENATE("0x",DEC2HEX(_xlfn.BITAND(A6,127)))</f>
-        <v>0x13</v>
-      </c>
-      <c r="N24" s="21"/>
-      <c r="P24" s="6" t="str">
-        <f>X21</f>
-        <v/>
-      </c>
-      <c r="Q24" t="str">
-        <f>Y21</f>
-        <v/>
-      </c>
-      <c r="S24" t="str">
-        <f>IF(P28, CONCATENATE("PC+4 = 0x", DEC2HEX(A8+4)," ",IF(K24=0,"NOT ", ""),"written to R",K24), "")</f>
-        <v/>
-      </c>
-      <c r="U24" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="V24" s="26"/>
-      <c r="W24" s="26"/>
-    </row>
-    <row r="26" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I27" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="J27" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="K27" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="L27" s="31"/>
-      <c r="M27" s="12" t="s">
+      <c r="M27" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N27" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="O27" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="N27" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="O27" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="P27" s="12" t="s">
+      <c r="P27" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="R27" s="33"/>
-    </row>
-    <row r="28" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="13" t="b">
+      <c r="Q27" s="19"/>
+    </row>
+    <row r="28" spans="3:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="12" t="b">
         <f>AND((M8=0),(N8&lt;&gt;7),(O8=3))</f>
         <v>0</v>
       </c>
-      <c r="D28" s="13" t="b">
+      <c r="D28" s="12" t="b">
         <f>AND((M8=3),(N8&lt;&gt;7),(O8=3))</f>
         <v>0</v>
       </c>
-      <c r="E28" s="32" t="b">
+      <c r="E28" s="47" t="b">
         <f>AND((M8=4),(N8&lt;&gt;7),(O8=3))</f>
-        <v>1</v>
-      </c>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F28" s="48"/>
+      <c r="G28" s="18" t="b">
         <f>AND((M8=5),(N8&lt;&gt;7),(O8=3))</f>
         <v>0</v>
       </c>
-      <c r="I28" s="13" t="b">
+      <c r="H28" s="18" t="b">
         <f>AND((M8=8),(N8&lt;&gt;7),(O8=3))</f>
-        <v>0</v>
-      </c>
-      <c r="J28" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="18" t="b">
         <f>AND((M8=11),(N8&lt;&gt;7),(O8=3))</f>
         <v>0</v>
       </c>
-      <c r="K28" s="32" t="b">
-        <f>AND((B8=12),(M8&lt;&gt;7),(N8=3))</f>
+      <c r="J28" s="47" t="b">
+        <f>AND((M8=12),(N8&lt;&gt;7),(O8=3),_xlfn.BITRSHIFT(HEX2DEC(A2),25)=0)</f>
         <v>0</v>
       </c>
-      <c r="L28" s="32"/>
-      <c r="M28" s="13" t="b">
+      <c r="K28" s="48"/>
+      <c r="L28" s="18" t="b">
         <f>AND((M8=13),(N8&lt;&gt;7),(O8=3))</f>
         <v>0</v>
       </c>
-      <c r="N28" s="13" t="b">
+      <c r="M28" s="18" t="b">
         <f>AND((M8=24),(N8&lt;&gt;7),(O8=3))</f>
         <v>0</v>
       </c>
-      <c r="O28" s="13" t="b">
+      <c r="N28" s="18" t="b">
         <f>AND((M8=25),(N8&lt;&gt;7),(O8=3))</f>
         <v>0</v>
       </c>
-      <c r="P28" s="13" t="b">
+      <c r="O28" s="18" t="b">
         <f>AND((M8=27),(N8&lt;&gt;7),(O8=3))</f>
         <v>0</v>
       </c>
-      <c r="Q28" s="32" t="b">
+      <c r="P28" s="47" t="b">
         <f>AND((M8=28),(N8&lt;&gt;7),(O8=3))</f>
         <v>0</v>
       </c>
-      <c r="R28" s="32"/>
-    </row>
-    <row r="31" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
+      <c r="Q28" s="48"/>
+    </row>
+    <row r="31" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="66">
-    <mergeCell ref="U22:W22"/>
-    <mergeCell ref="U23:W23"/>
-    <mergeCell ref="U24:W24"/>
-    <mergeCell ref="U7:W7"/>
-    <mergeCell ref="U8:W8"/>
-    <mergeCell ref="U9:W9"/>
-    <mergeCell ref="U10:W10"/>
-    <mergeCell ref="U11:W11"/>
-    <mergeCell ref="U12:W12"/>
-    <mergeCell ref="U13:W13"/>
-    <mergeCell ref="U14:W14"/>
-    <mergeCell ref="U15:W15"/>
+  <mergeCells count="73">
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="O11:R11"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="T24:V24"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="O14:R14"/>
+    <mergeCell ref="O17:R17"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="O23:R23"/>
     <mergeCell ref="U16:W16"/>
+    <mergeCell ref="Q15:S15"/>
     <mergeCell ref="U17:W17"/>
     <mergeCell ref="U18:W18"/>
     <mergeCell ref="U19:W19"/>
-    <mergeCell ref="U20:W20"/>
-    <mergeCell ref="U21:W21"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="Q27:R27"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="H18:I18"/>
@@ -1816,13 +2233,11 @@
     <mergeCell ref="M24:N24"/>
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K20:L20"/>
     <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H14:I14"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D21:J21"/>
@@ -1831,96 +2246,134 @@
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="D14:G14"/>
     <mergeCell ref="D15:G15"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H14:I14"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="H23:J23"/>
     <mergeCell ref="H24:J24"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="U9:W9"/>
+    <mergeCell ref="U8:W8"/>
+    <mergeCell ref="U7:W7"/>
+    <mergeCell ref="U6:W6"/>
+    <mergeCell ref="U4:W4"/>
+    <mergeCell ref="U14:W14"/>
+    <mergeCell ref="U13:W13"/>
+    <mergeCell ref="U12:W12"/>
+    <mergeCell ref="U11:W11"/>
+    <mergeCell ref="U10:W10"/>
+    <mergeCell ref="U15:W15"/>
   </mergeCells>
-  <conditionalFormatting sqref="E28:G28">
-    <cfRule type="cellIs" dxfId="0" priority="15" operator="equal">
+  <conditionalFormatting sqref="E28">
+    <cfRule type="cellIs" dxfId="36" priority="8" operator="equal">
+      <formula>"E28"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="20" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="21" operator="equal">
       <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"E28"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="cellIs" dxfId="26" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="19" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="18" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28">
+    <cfRule type="cellIs" dxfId="31" priority="17" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="cellIs" dxfId="24" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28">
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="15" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28">
-    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K28:L28">
-    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
+  <conditionalFormatting sqref="L28">
+    <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M28">
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N28">
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="11" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O28">
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P28">
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q28:R28">
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
-      <formula>TRUE</formula>
+  <conditionalFormatting sqref="U5">
+    <cfRule type="expression" priority="6">
+      <formula>E28=TRUE</formula>
+    </cfRule>
+    <cfRule type="expression" priority="7">
+      <formula>"E28=TRUE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U10:W10">
-    <cfRule type="expression" priority="2">
-      <formula>"E28=TRUE"</formula>
+  <conditionalFormatting sqref="O14">
+    <cfRule type="containsText" dxfId="22" priority="5" operator="containsText" text="&lt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;",O14)))</formula>
     </cfRule>
-    <cfRule type="expression" priority="1">
-      <formula>E28=TRUE</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O17">
+    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="&lt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;",O17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="&lt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;",O17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O23">
+    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="&lt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;",O23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O11:R11">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&lt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;",O11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fetch branch predecode fix, execute fix, decoding spreadsheet Bxx addition
</commit_message>
<xml_diff>
--- a/RISC-V_decode.xlsx
+++ b/RISC-V_decode.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="65">
   <si>
     <t>RV32I</t>
   </si>
@@ -201,13 +201,28 @@
   </si>
   <si>
     <t>007F4533</t>
+  </si>
+  <si>
+    <t>B-type</t>
+  </si>
+  <si>
+    <t>31-imm[12|10:5] -25</t>
+  </si>
+  <si>
+    <t>11 -  imm[4:1|11] - 7</t>
+  </si>
+  <si>
+    <t>Enter Decimal value</t>
+  </si>
+  <si>
+    <t>Hexadecimal Equivalent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,8 +273,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,8 +385,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -541,16 +574,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -578,9 +621,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="4"/>
@@ -594,78 +634,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -685,6 +653,78 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -694,14 +734,14 @@
     <xf numFmtId="0" fontId="6" fillId="18" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -712,19 +752,51 @@
     <xf numFmtId="0" fontId="6" fillId="17" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="7" xfId="6" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="6" builtinId="20"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="5" builtinId="10"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="39">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -903,6 +975,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="6" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFCC00"/>
         </patternFill>
       </fill>
@@ -995,56 +1074,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1426,10 +1455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y31"/>
+  <dimension ref="A1:Z31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U23" sqref="U23"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,17 +1482,17 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="T2" t="s">
         <v>51</v>
       </c>
-      <c r="U2" s="17" t="s">
+      <c r="U2" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="V2" s="17"/>
-      <c r="W2" s="17"/>
-      <c r="X2" s="20"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="19"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1481,18 +1510,18 @@
       <c r="T3" t="s">
         <v>49</v>
       </c>
-      <c r="U3" s="21" t="s">
+      <c r="U3" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="22"/>
-      <c r="W3" s="23"/>
-      <c r="X3" s="20" t="str">
-        <f>IF(C28,   IF(J15=0,"LB",(IF(J15=1,"LH",(IF(J15=2,"LW",IF(J15=4,"LBU",IF(J15=5,"LHU"," "))))))), " ")</f>
-        <v xml:space="preserve"> </v>
+      <c r="V3" s="49"/>
+      <c r="W3" s="50"/>
+      <c r="X3" s="19" t="str">
+        <f>IF(C31,   IF(J15=0,"LB",(IF(J15=1,"LH",(IF(J15=2,"LW",IF(J15=4,"LBU",IF(J15=5,"LHU"," "))))))), " ")</f>
+        <v>LW</v>
       </c>
       <c r="Y3" t="str">
-        <f>IF(C28, CONCATENATE("X",K15,", 0x",DEC2HEX(D15),"(X",H15,")"), " ")</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(C31, CONCATENATE("X",K15,", 0x",DEC2HEX(D15),"(X",H15,")"), " ")</f>
+        <v>X14, 0xFEC(X8)</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -1500,7 +1529,7 @@
         <v>42</v>
       </c>
       <c r="C4" t="b">
-        <f>OR(C28,D28,E28,G28,H28,I28,K28,L28,M28,N28,O28,P28)</f>
+        <f>OR(C31,D31,E31,G31,H31,I31,K31,L31,M31,N31,O31,P31)</f>
         <v>1</v>
       </c>
       <c r="D4" t="b">
@@ -1511,41 +1540,41 @@
         <f>NOT(OR(C4,D4))</f>
         <v>0</v>
       </c>
-      <c r="U4" s="25" t="s">
+      <c r="U4" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="V4" s="26"/>
-      <c r="W4" s="27"/>
-      <c r="X4" s="20" t="str">
-        <f>IF(D28, "Fence", "")</f>
+      <c r="V4" s="55"/>
+      <c r="W4" s="56"/>
+      <c r="X4" s="19" t="str">
+        <f>IF(D31, "Fence", "")</f>
         <v/>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>5</v>
       </c>
       <c r="T5" t="s">
         <v>50</v>
       </c>
-      <c r="U5" s="21" t="s">
+      <c r="U5" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="V5" s="22"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="20" t="str">
-        <f>IF(E28,IF(K15,IF(J15=0,"ADDI",IF(J15=1,"SLLI",IF(J15=2,"SLTI",IF(J15=3,"SLTIU",IF(J15=4,"XORI",IF(AND(J15=5,D12=0),"SRLI",IF(AND(J15=5,D12=32),"SRAI",IF(J15=6,"ORI",IF(J15=7,"ANDI"," ")))))))))), " ")</f>
+      <c r="V5" s="49"/>
+      <c r="W5" s="50"/>
+      <c r="X5" s="19" t="str">
+        <f>IF(E31,IF(K15,IF(J15=0,"ADDI",IF(J15=1,"SLLI",IF(J15=2,"SLTI",IF(J15=3,"SLTIU",IF(J15=4,"XORI",IF(AND(J15=5,D12=0),"SRLI",IF(AND(J15=5,D12=32),"SRAI",IF(J15=6,"ORI",IF(J15=7,"ANDI"," ")))))))))), " ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y5" t="str">
-        <f>IF(E28, CONCATENATE("X",K15,", X",H15,", 0x",D15), " ")</f>
+        <f>IF(E31, CONCATENATE("X",K15,", X",H15,", 0x",D15), " ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>HEX2DEC(A2)</f>
-        <v>4277412899</v>
+        <v>4274267907</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>8</v>
@@ -1556,15 +1585,15 @@
       <c r="O6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U6" s="25" t="s">
+      <c r="U6" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="V6" s="26"/>
-      <c r="W6" s="27"/>
-      <c r="X6" s="20"/>
+      <c r="V6" s="55"/>
+      <c r="W6" s="56"/>
+      <c r="X6" s="19"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>35</v>
       </c>
       <c r="L7" s="4" t="s">
@@ -1572,7 +1601,7 @@
       </c>
       <c r="M7" s="4" t="str">
         <f>DEC2BIN(M8)</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N7" s="4" t="str">
         <f>DEC2BIN(N8)</f>
@@ -1585,18 +1614,18 @@
       <c r="T7" t="s">
         <v>47</v>
       </c>
-      <c r="U7" s="58" t="s">
+      <c r="U7" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="V7" s="59"/>
-      <c r="W7" s="60"/>
-      <c r="X7" s="45" t="str">
-        <f>IF(H28, IF(J18=0,"SB",IF(J18=1,"SH",IF(J18=2,"SW"," ")))," ")</f>
-        <v>SW</v>
+      <c r="V7" s="58"/>
+      <c r="W7" s="59"/>
+      <c r="X7" s="20" t="str">
+        <f>IF(H31, IF(J18=0,"SB",IF(J18=1,"SH",IF(J18=2,"SW"," ")))," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="Y7" t="str">
-        <f>IF(H28,CONCATENATE("X",F18,", 0x",DEC2HEX(_xlfn.BITLSHIFT(D18,5)+K18),"(X",H18,")")," ")</f>
-        <v>X15, 0xFE8(X8)</v>
+        <f>IF(H31,CONCATENATE("X",F18,", 0x",DEC2HEX(_xlfn.BITLSHIFT(D18,5)+K18),"(X",H18,")")," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -1609,7 +1638,7 @@
       </c>
       <c r="M8">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,2),31)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="N8">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,2),7)</f>
@@ -1619,28 +1648,28 @@
         <f>_xlfn.BITAND(A6,3)</f>
         <v>3</v>
       </c>
-      <c r="U8" s="25" t="s">
+      <c r="U8" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="V8" s="26"/>
-      <c r="W8" s="27"/>
-      <c r="X8" s="20"/>
+      <c r="V8" s="55"/>
+      <c r="W8" s="56"/>
+      <c r="X8" s="19"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="T9" t="s">
         <v>59</v>
       </c>
-      <c r="U9" s="52" t="s">
+      <c r="U9" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="V9" s="53"/>
-      <c r="W9" s="54"/>
-      <c r="X9" s="45" t="str">
-        <f>IF(J28, IF(D12=0,IF(J12=0,"ADD",IF(J12=1, "SLL",IF(J12=2,"SLT",IF(J12=3,"SLTU",IF(J12=4,"XOR",IF(J12=5,"SRL",IF(J12=6,"OR",IF(J12=7,"AND", " ")))))))), IF(D12=BIN2DEC(100000), IF(J12=0,"SUB",IF(J12=1,"SRA", " ")))), " ")</f>
+      <c r="V9" s="52"/>
+      <c r="W9" s="53"/>
+      <c r="X9" s="20" t="str">
+        <f>IF(J31, IF(D12=0,IF(J12=0,"ADD",IF(J12=1, "SLL",IF(J12=2,"SLT",IF(J12=3,"SLTU",IF(J12=4,"XOR",IF(J12=5,"SRL",IF(J12=6,"OR",IF(J12=7,"AND", " ")))))))), IF(D12=BIN2DEC(100000), IF(J12=0,"SUB",IF(J12=1,"SRA", " ")))), " ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y9" t="str">
-        <f>IF(J28, CONCATENATE("R",K12,", R",H12," ,R",F12), " ")</f>
+        <f>IF(J31, CONCATENATE("R",K12,", R",H12," ,R",F12), " ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -1648,22 +1677,22 @@
       <c r="C10" t="s">
         <v>29</v>
       </c>
-      <c r="U10" s="25" t="s">
+      <c r="U10" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="V10" s="26"/>
-      <c r="W10" s="27"/>
-      <c r="X10" s="20"/>
+      <c r="V10" s="55"/>
+      <c r="W10" s="56"/>
+      <c r="X10" s="19"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="33" t="s">
+      <c r="E11" s="43"/>
+      <c r="F11" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="33"/>
+      <c r="G11" s="39"/>
       <c r="H11" s="34" t="s">
         <v>55</v>
       </c>
@@ -1671,77 +1700,77 @@
       <c r="J11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="38" t="s">
+      <c r="K11" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="L11" s="38"/>
-      <c r="M11" s="55" t="s">
+      <c r="L11" s="37"/>
+      <c r="M11" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="N11" s="55"/>
-      <c r="O11" s="56" t="str">
-        <f>IF(J28," &lt;---- Integer Register Register format"," ")</f>
+      <c r="N11" s="44"/>
+      <c r="O11" s="27" t="str">
+        <f>IF(J31," &lt;---- Integer Register Register format"," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P11" s="56"/>
-      <c r="Q11" s="56"/>
-      <c r="R11" s="56"/>
-      <c r="U11" s="25" t="s">
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+      <c r="U11" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="V11" s="26"/>
-      <c r="W11" s="27"/>
-      <c r="X11" s="20"/>
+      <c r="V11" s="55"/>
+      <c r="W11" s="56"/>
+      <c r="X11" s="19"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="32">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,25),127)</f>
         <v>127</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="29">
+      <c r="E12" s="33"/>
+      <c r="F12" s="32">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,20),15)</f>
-        <v>15</v>
-      </c>
-      <c r="G12" s="30"/>
-      <c r="H12" s="29">
+        <v>12</v>
+      </c>
+      <c r="G12" s="33"/>
+      <c r="H12" s="32">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,15),31)</f>
         <v>8</v>
       </c>
-      <c r="I12" s="30"/>
+      <c r="I12" s="33"/>
       <c r="J12" s="7">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,12),7)</f>
         <v>2</v>
       </c>
-      <c r="K12" s="29">
+      <c r="K12" s="32">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,7),31)</f>
-        <v>8</v>
-      </c>
-      <c r="L12" s="30"/>
-      <c r="M12" s="29" t="str">
+        <v>14</v>
+      </c>
+      <c r="L12" s="33"/>
+      <c r="M12" s="32" t="str">
         <f>CONCATENATE("0x",DEC2HEX(_xlfn.BITAND(A6,127)))</f>
-        <v>0x23</v>
-      </c>
-      <c r="N12" s="30"/>
+        <v>0x3</v>
+      </c>
+      <c r="N12" s="33"/>
       <c r="P12" s="6" t="str">
-        <f>IF(J28, X9, " ")</f>
+        <f>X9</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Q12" s="24" t="str">
+      <c r="Q12" s="28" t="str">
         <f>Y9</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="U12" s="25" t="s">
+      <c r="R12" s="28"/>
+      <c r="S12" s="28"/>
+      <c r="U12" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="V12" s="26"/>
-      <c r="W12" s="27"/>
-      <c r="X12" s="20"/>
+      <c r="V12" s="55"/>
+      <c r="W12" s="56"/>
+      <c r="X12" s="19"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D13" s="8"/>
@@ -1755,20 +1784,20 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
-      <c r="U13" s="25" t="s">
+      <c r="U13" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="V13" s="26"/>
-      <c r="W13" s="27"/>
-      <c r="X13" s="20"/>
+      <c r="V13" s="55"/>
+      <c r="W13" s="56"/>
+      <c r="X13" s="19"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
       <c r="H14" s="34" t="s">
         <v>55</v>
       </c>
@@ -1776,82 +1805,92 @@
       <c r="J14" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K14" s="51" t="s">
+      <c r="K14" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="L14" s="51"/>
-      <c r="M14" s="44" t="s">
+      <c r="L14" s="26"/>
+      <c r="M14" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="N14" s="44"/>
-      <c r="O14" s="24" t="str">
-        <f>IF(C28,"  &lt;---- Load Instruction format", IF(E28,"  &lt;---- Arithmetic Immediate format",  IF(N28,"  &lt;---- JALR format"," ")))</f>
+      <c r="N14" s="45"/>
+      <c r="O14" s="28" t="str">
+        <f>IF(C31,"  &lt;---- Load Instruction format", IF(E31,"  &lt;---- Arithmetic Immediate format",  IF(N31,"  &lt;---- JALR format"," ")))</f>
+        <v xml:space="preserve">  &lt;---- Load Instruction format</v>
+      </c>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="T14">
+        <v>8063</v>
+      </c>
+      <c r="U14" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="V14" s="64"/>
+      <c r="W14" s="65"/>
+      <c r="X14" s="20" t="str">
+        <f>IF(M31, IF(J27=0, "BEQ", IF(J27=1,"BNE", IF(J27=4,"BLT", IF(J27=5,"BGE", IF(J27=6,"BLTU", IF(J27=7, "BGEU", " "))))))," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="U14" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="V14" s="26"/>
-      <c r="W14" s="27"/>
-      <c r="X14" s="20"/>
+      <c r="Y14" t="str">
+        <f>IF(M31,CONCATENATE("R",H27,", R",F27," , 0x", DEC2HEX( _xlfn.BITAND(_xlfn.BITRSHIFT(K27,8),15)*2 + _xlfn.BITAND(_xlfn.BITRSHIFT(D27,25),63)*32 + _xlfn.BITAND(_xlfn.BITRSHIFT(K27,7),1)*2048 + _xlfn.BITLSHIFT(_xlfn.BITAND(_xlfn.BITRSHIFT(D27,31),1),31)  )), " ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="32">
         <f>(_xlfn.BITAND(_xlfn.BITRSHIFT(A6,20),4095))</f>
-        <v>4079</v>
-      </c>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="29">
+        <v>4076</v>
+      </c>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="32">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,15),31)</f>
         <v>8</v>
       </c>
-      <c r="I15" s="30"/>
+      <c r="I15" s="33"/>
       <c r="J15" s="7">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,12),7)</f>
         <v>2</v>
       </c>
-      <c r="K15" s="29">
+      <c r="K15" s="32">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,7),31)</f>
-        <v>8</v>
-      </c>
-      <c r="L15" s="30"/>
-      <c r="M15" s="29" t="str">
+        <v>14</v>
+      </c>
+      <c r="L15" s="33"/>
+      <c r="M15" s="32" t="str">
         <f>CONCATENATE("0x",DEC2HEX(_xlfn.BITAND(A6,127)))</f>
-        <v>0x23</v>
-      </c>
-      <c r="N15" s="30"/>
+        <v>0x3</v>
+      </c>
+      <c r="N15" s="33"/>
       <c r="P15" s="6" t="str">
-        <f>IF(C28, X3, IF(E28,X5,IF(N28,X15," ")))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="Q15" s="24" t="str">
-        <f>IF(C28, Y3, IF(E28, Y5,IF(N28,Y15," ")))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
+        <f>IF(C31, X3, IF(E31,X5,IF(N31,X15," ")))</f>
+        <v>LW</v>
+      </c>
+      <c r="Q15" s="28" t="str">
+        <f>IF(C31, Y3, IF(E31, Y5,IF(N31,Y15," ")))</f>
+        <v>X14, 0xFEC(X8)</v>
+      </c>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
       <c r="T15" t="s">
         <v>46</v>
       </c>
-      <c r="U15" s="40" t="s">
+      <c r="U15" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="V15" s="40"/>
-      <c r="W15" s="40"/>
-      <c r="X15" s="20" t="str">
-        <f>IF(N28,  "JALR", " ")</f>
+      <c r="V15" s="60"/>
+      <c r="W15" s="60"/>
+      <c r="X15" s="19" t="str">
+        <f>IF(N31,  "JALR", " ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y15" t="str">
-        <f>IF(N28,CONCATENATE("R",K15,", 0x",DEC2HEX(D15),"(R",H15,")"),"")</f>
+        <f>IF(N31,CONCATENATE("R",K15,", 0x",DEC2HEX(D15),"(R",H15,")"),"")</f>
         <v/>
       </c>
     </row>
@@ -1863,29 +1902,29 @@
       <c r="T16" t="s">
         <v>48</v>
       </c>
-      <c r="U16" s="41" t="s">
+      <c r="U16" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="V16" s="41"/>
-      <c r="W16" s="41"/>
-      <c r="X16" s="20" t="str">
-        <f>IF(O28,  "JAL", " ")</f>
+      <c r="V16" s="30"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="19" t="str">
+        <f>IF(O31,  "JAL", " ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y16" t="str">
-        <f>IF(O28, CONCATENATE("X",K24,", 0x", DEC2HEX(_xlfn.BITLSHIFT(E24,1)+_xlfn.BITLSHIFT(G24,11)+_xlfn.BITLSHIFT(H24,12)+_xlfn.BITLSHIFT(IF(D24, 4095,0),20)+A8)), "")</f>
+        <f>IF(O31, CONCATENATE("X",K24,", 0x", DEC2HEX(_xlfn.BITLSHIFT(E24,1)+_xlfn.BITLSHIFT(G24,11)+_xlfn.BITLSHIFT(H24,12)+_xlfn.BITLSHIFT(IF(D24, 4095,0),20)+A8)), "")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="D17" s="35" t="s">
+    <row r="17" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="D17" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="35"/>
-      <c r="F17" s="33" t="s">
+      <c r="E17" s="40"/>
+      <c r="F17" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="33"/>
+      <c r="G17" s="39"/>
       <c r="H17" s="34" t="s">
         <v>55</v>
       </c>
@@ -1893,348 +1932,452 @@
       <c r="J17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K17" s="39" t="s">
+      <c r="K17" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="L17" s="39"/>
-      <c r="M17" s="57" t="s">
+      <c r="L17" s="47"/>
+      <c r="M17" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="N17" s="57"/>
-      <c r="O17" s="61" t="str">
-        <f>IF(H28,"  &lt;---- Store Instruction format"," ")</f>
-        <v xml:space="preserve">  &lt;---- Store Instruction format</v>
-      </c>
-      <c r="P17" s="61"/>
-      <c r="Q17" s="61"/>
-      <c r="R17" s="61"/>
-      <c r="U17" s="42" t="s">
+      <c r="N17" s="46"/>
+      <c r="O17" s="29" t="str">
+        <f>IF(H31,"  &lt;---- Store Instruction format"," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="U17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="V17" s="42"/>
-      <c r="W17" s="42"/>
-      <c r="X17" s="20"/>
-    </row>
-    <row r="18" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="V17" s="31"/>
+      <c r="W17" s="31"/>
+      <c r="X17" s="19"/>
+    </row>
+    <row r="18" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="32">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,25),127)</f>
         <v>127</v>
       </c>
-      <c r="E18" s="30"/>
-      <c r="F18" s="29">
+      <c r="E18" s="33"/>
+      <c r="F18" s="32">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,20),15)</f>
-        <v>15</v>
-      </c>
-      <c r="G18" s="30"/>
-      <c r="H18" s="29">
+        <v>12</v>
+      </c>
+      <c r="G18" s="33"/>
+      <c r="H18" s="32">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,15),31)</f>
         <v>8</v>
       </c>
-      <c r="I18" s="30"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="7">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,12),7)</f>
         <v>2</v>
       </c>
-      <c r="K18" s="29">
+      <c r="K18" s="32">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,7),15)</f>
-        <v>8</v>
-      </c>
-      <c r="L18" s="30"/>
-      <c r="M18" s="29" t="str">
+        <v>14</v>
+      </c>
+      <c r="L18" s="33"/>
+      <c r="M18" s="32" t="str">
         <f>CONCATENATE("0x",DEC2HEX(_xlfn.BITAND(A6,127)))</f>
-        <v>0x23</v>
-      </c>
-      <c r="N18" s="30"/>
+        <v>0x3</v>
+      </c>
+      <c r="N18" s="33"/>
       <c r="P18" s="6" t="str">
         <f>X7</f>
-        <v>SW</v>
-      </c>
-      <c r="Q18" s="24" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Q18" s="28" t="str">
         <f>Y7</f>
-        <v>X15, 0xFE8(X8)</v>
-      </c>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
-      <c r="U18" s="42" t="s">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
+      <c r="U18" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="V18" s="42"/>
-      <c r="W18" s="42"/>
-      <c r="X18" s="20"/>
-    </row>
-    <row r="19" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="U19" s="42" t="s">
+      <c r="V18" s="31"/>
+      <c r="W18" s="31"/>
+      <c r="X18" s="19"/>
+    </row>
+    <row r="19" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="U19" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="V19" s="42"/>
-      <c r="W19" s="42"/>
-      <c r="X19" s="20"/>
-    </row>
-    <row r="20" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="D20" s="31" t="s">
+      <c r="V19" s="31"/>
+      <c r="W19" s="31"/>
+      <c r="X19" s="19"/>
+    </row>
+    <row r="20" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="D20" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="38" t="s">
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="L20" s="38"/>
-      <c r="M20" s="28" t="s">
+      <c r="L20" s="37"/>
+      <c r="M20" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="N20" s="28"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-    </row>
-    <row r="21" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="N20" s="35"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="28"/>
+    </row>
+    <row r="21" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="29">
+      <c r="D21" s="32">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,12),1048575)</f>
-        <v>1044290</v>
-      </c>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="29">
+        <v>1043522</v>
+      </c>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="32">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,7),31)</f>
-        <v>8</v>
-      </c>
-      <c r="L21" s="30"/>
-      <c r="M21" s="29" t="str">
+        <v>14</v>
+      </c>
+      <c r="L21" s="33"/>
+      <c r="M21" s="32" t="str">
         <f>CONCATENATE("0x",DEC2HEX(_xlfn.BITAND(A6,127)))</f>
-        <v>0x23</v>
-      </c>
-      <c r="N21" s="30"/>
-    </row>
-    <row r="23" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="D23" s="14" t="s">
+        <v>0x3</v>
+      </c>
+      <c r="N21" s="33"/>
+    </row>
+    <row r="23" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="D23" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="31"/>
-      <c r="G23" s="14" t="s">
+      <c r="F23" s="38"/>
+      <c r="G23" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H23" s="31" t="s">
+      <c r="H23" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="38" t="s">
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="L23" s="38"/>
-      <c r="M23" s="43" t="s">
+      <c r="L23" s="37"/>
+      <c r="M23" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="N23" s="43"/>
-      <c r="O23" s="24" t="str">
-        <f>IF(O28,"  &lt;---- JAL format"," ")</f>
+      <c r="N23" s="36"/>
+      <c r="O23" s="28" t="str">
+        <f>IF(O31,"  &lt;---- JAL format"," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="24"/>
-    </row>
-    <row r="24" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="P23" s="28"/>
+      <c r="Q23" s="28"/>
+      <c r="R23" s="28"/>
+    </row>
+    <row r="24" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="14">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,31),1)</f>
         <v>1</v>
       </c>
-      <c r="E24" s="29">
+      <c r="E24" s="32">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,21),1023)</f>
-        <v>1015</v>
-      </c>
-      <c r="F24" s="30"/>
-      <c r="G24" s="15">
+        <v>1014</v>
+      </c>
+      <c r="F24" s="33"/>
+      <c r="G24" s="14">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,20),1)</f>
-        <v>1</v>
-      </c>
-      <c r="H24" s="29">
+        <v>0</v>
+      </c>
+      <c r="H24" s="32">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,12),255)</f>
         <v>66</v>
       </c>
-      <c r="I24" s="32"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="29">
+      <c r="I24" s="41"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="32">
         <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,7),31)</f>
-        <v>8</v>
-      </c>
-      <c r="L24" s="30"/>
-      <c r="M24" s="29" t="str">
+        <v>14</v>
+      </c>
+      <c r="L24" s="33"/>
+      <c r="M24" s="32" t="str">
         <f>CONCATENATE("0x",DEC2HEX(_xlfn.BITAND(A6,127)))</f>
-        <v>0x23</v>
-      </c>
-      <c r="N24" s="30"/>
+        <v>0x3</v>
+      </c>
+      <c r="N24" s="33"/>
       <c r="P24" s="6" t="str">
         <f>X16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Q24" s="24" t="str">
+      <c r="Q24" s="28" t="str">
         <f>Y16</f>
         <v/>
       </c>
-      <c r="R24" s="24"/>
-      <c r="S24" s="24"/>
-      <c r="T24" s="24" t="str">
-        <f>IF(O28, CONCATENATE("PC+4 = 0x", DEC2HEX(A8+4)," ",IF(K24=0,"NOT ", ""),"written to X",K24), "")</f>
+      <c r="R24" s="28"/>
+      <c r="S24" s="28"/>
+      <c r="T24" s="28" t="str">
+        <f>IF(O31, CONCATENATE("PC+4 = 0x", DEC2HEX(A8+4)," ",IF(K24=0,"NOT ", ""),"written to X",K24), "")</f>
         <v/>
       </c>
-      <c r="U24" s="24"/>
-      <c r="V24" s="24"/>
-    </row>
-    <row r="26" spans="3:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="3:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="11" t="s">
+      <c r="U24" s="28"/>
+      <c r="V24" s="28"/>
+    </row>
+    <row r="26" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="D26" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="61"/>
+      <c r="F26" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" s="39"/>
+      <c r="H26" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="I26" s="34"/>
+      <c r="J26" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="L26" s="47"/>
+      <c r="M26" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="N26" s="62"/>
+      <c r="O26" s="27" t="str">
+        <f>IF(M31,"  &lt;----Bxx Instruction format"," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="27"/>
+    </row>
+    <row r="27" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="32">
+        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,25),127)</f>
+        <v>127</v>
+      </c>
+      <c r="E27" s="33"/>
+      <c r="F27" s="32">
+        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,20),15)</f>
+        <v>12</v>
+      </c>
+      <c r="G27" s="33"/>
+      <c r="H27" s="32">
+        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,15),31)</f>
+        <v>8</v>
+      </c>
+      <c r="I27" s="33"/>
+      <c r="J27" s="7">
+        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,12),7)</f>
+        <v>2</v>
+      </c>
+      <c r="K27" s="32">
+        <f>_xlfn.BITAND(_xlfn.BITRSHIFT(A6,7),15)</f>
+        <v>14</v>
+      </c>
+      <c r="L27" s="33"/>
+      <c r="M27" s="32" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(_xlfn.BITAND(A6,127)))</f>
+        <v>0x3</v>
+      </c>
+      <c r="N27" s="33"/>
+      <c r="P27" s="6" t="str">
+        <f xml:space="preserve"> X14</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Q27" s="28" t="str">
+        <f>Y14</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="R27" s="28"/>
+      <c r="S27" s="28"/>
+    </row>
+    <row r="29" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D30" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="46" t="s">
+      <c r="E30" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="F27" s="46"/>
-      <c r="G27" s="11" t="s">
+      <c r="F30" s="21"/>
+      <c r="G30" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H30" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I27" s="11" t="s">
+      <c r="I30" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J27" s="49" t="s">
+      <c r="J30" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="K27" s="50"/>
-      <c r="L27" s="11" t="s">
+      <c r="K30" s="25"/>
+      <c r="L30" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="11" t="s">
+      <c r="M30" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="N27" s="11" t="s">
+      <c r="N30" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="O27" s="11" t="s">
+      <c r="O30" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="P27" s="19" t="s">
+      <c r="P30" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="19"/>
-    </row>
-    <row r="28" spans="3:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="12" t="b">
+      <c r="Q30" s="18"/>
+      <c r="U30" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="V30" s="67"/>
+      <c r="W30" s="67"/>
+      <c r="X30" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y30" s="66"/>
+      <c r="Z30" s="66"/>
+    </row>
+    <row r="31" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="12" t="b">
         <f>AND((M8=0),(N8&lt;&gt;7),(O8=3))</f>
-        <v>0</v>
-      </c>
-      <c r="D28" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="12" t="b">
         <f>AND((M8=3),(N8&lt;&gt;7),(O8=3))</f>
         <v>0</v>
       </c>
-      <c r="E28" s="47" t="b">
+      <c r="E31" s="22" t="b">
         <f>AND((M8=4),(N8&lt;&gt;7),(O8=3))</f>
         <v>0</v>
       </c>
-      <c r="F28" s="48"/>
-      <c r="G28" s="18" t="b">
+      <c r="F31" s="23"/>
+      <c r="G31" s="17" t="b">
         <f>AND((M8=5),(N8&lt;&gt;7),(O8=3))</f>
         <v>0</v>
       </c>
-      <c r="H28" s="18" t="b">
+      <c r="H31" s="17" t="b">
         <f>AND((M8=8),(N8&lt;&gt;7),(O8=3))</f>
-        <v>1</v>
-      </c>
-      <c r="I28" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" s="17" t="b">
         <f>AND((M8=11),(N8&lt;&gt;7),(O8=3))</f>
         <v>0</v>
       </c>
-      <c r="J28" s="47" t="b">
+      <c r="J31" s="22" t="b">
         <f>AND((M8=12),(N8&lt;&gt;7),(O8=3),_xlfn.BITRSHIFT(HEX2DEC(A2),25)=0)</f>
         <v>0</v>
       </c>
-      <c r="K28" s="48"/>
-      <c r="L28" s="18" t="b">
+      <c r="K31" s="23"/>
+      <c r="L31" s="17" t="b">
         <f>AND((M8=13),(N8&lt;&gt;7),(O8=3))</f>
         <v>0</v>
       </c>
-      <c r="M28" s="18" t="b">
+      <c r="M31" s="17" t="b">
         <f>AND((M8=24),(N8&lt;&gt;7),(O8=3))</f>
         <v>0</v>
       </c>
-      <c r="N28" s="18" t="b">
+      <c r="N31" s="17" t="b">
         <f>AND((M8=25),(N8&lt;&gt;7),(O8=3))</f>
         <v>0</v>
       </c>
-      <c r="O28" s="18" t="b">
+      <c r="O31" s="17" t="b">
         <f>AND((M8=27),(N8&lt;&gt;7),(O8=3))</f>
         <v>0</v>
       </c>
-      <c r="P28" s="47" t="b">
+      <c r="P31" s="22" t="b">
         <f>AND((M8=28),(N8&lt;&gt;7),(O8=3))</f>
         <v>0</v>
       </c>
-      <c r="Q28" s="48"/>
-    </row>
-    <row r="31" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
+      <c r="Q31" s="23"/>
+      <c r="U31" s="68">
+        <v>127</v>
+      </c>
+      <c r="V31" s="68"/>
+      <c r="W31" s="68"/>
+      <c r="X31" s="68" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(U31))</f>
+        <v>0x7F</v>
+      </c>
+      <c r="Y31" s="68"/>
+      <c r="Z31" s="68"/>
     </row>
   </sheetData>
-  <mergeCells count="73">
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="O11:R11"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="T24:V24"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="O14:R14"/>
-    <mergeCell ref="O17:R17"/>
-    <mergeCell ref="O20:R20"/>
-    <mergeCell ref="O23:R23"/>
-    <mergeCell ref="U16:W16"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="U18:W18"/>
-    <mergeCell ref="U19:W19"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="E23:F23"/>
+  <mergeCells count="89">
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="U30:W30"/>
+    <mergeCell ref="X30:Z30"/>
+    <mergeCell ref="U31:W31"/>
+    <mergeCell ref="X31:Z31"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="U12:W12"/>
+    <mergeCell ref="U11:W11"/>
+    <mergeCell ref="U10:W10"/>
+    <mergeCell ref="U15:W15"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="O26:R26"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="U9:W9"/>
+    <mergeCell ref="U8:W8"/>
+    <mergeCell ref="U7:W7"/>
+    <mergeCell ref="U6:W6"/>
+    <mergeCell ref="U4:W4"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K18:L18"/>
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="H14:I14"/>
@@ -2250,130 +2393,139 @@
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="D12:E12"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="U9:W9"/>
-    <mergeCell ref="U8:W8"/>
-    <mergeCell ref="U7:W7"/>
-    <mergeCell ref="U6:W6"/>
-    <mergeCell ref="U4:W4"/>
+    <mergeCell ref="O11:R11"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="T24:V24"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="O14:R14"/>
+    <mergeCell ref="O17:R17"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="U16:W16"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="U19:W19"/>
     <mergeCell ref="U14:W14"/>
     <mergeCell ref="U13:W13"/>
-    <mergeCell ref="U12:W12"/>
-    <mergeCell ref="U11:W11"/>
-    <mergeCell ref="U10:W10"/>
-    <mergeCell ref="U15:W15"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="E23:F23"/>
   </mergeCells>
-  <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="36" priority="8" operator="equal">
+  <conditionalFormatting sqref="E31">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
       <formula>"E28"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="22" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D28">
-    <cfRule type="cellIs" dxfId="33" priority="19" operator="equal">
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28">
-    <cfRule type="cellIs" dxfId="32" priority="18" operator="equal">
+  <conditionalFormatting sqref="C31">
+    <cfRule type="cellIs" dxfId="15" priority="19" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G28">
-    <cfRule type="cellIs" dxfId="31" priority="17" operator="equal">
+  <conditionalFormatting sqref="G31">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H28">
-    <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
+  <conditionalFormatting sqref="H31">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28">
-    <cfRule type="cellIs" dxfId="29" priority="15" operator="equal">
+  <conditionalFormatting sqref="I31">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J28">
-    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
+  <conditionalFormatting sqref="J31">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L28">
-    <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
+  <conditionalFormatting sqref="L31">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M28">
-    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
+  <conditionalFormatting sqref="M31">
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N28">
-    <cfRule type="cellIs" dxfId="25" priority="11" operator="equal">
+  <conditionalFormatting sqref="N31">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O28">
-    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
+  <conditionalFormatting sqref="O31">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P28">
-    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
+  <conditionalFormatting sqref="P31">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U5">
-    <cfRule type="expression" priority="6">
-      <formula>E28=TRUE</formula>
-    </cfRule>
-    <cfRule type="expression" priority="7">
-      <formula>"E28=TRUE"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="O14">
-    <cfRule type="containsText" dxfId="22" priority="5" operator="containsText" text="&lt;">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH("&lt;",O14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O17">
-    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="&lt;">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH("&lt;",O17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="&lt;">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH("&lt;",O17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O23">
-    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="&lt;">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH("&lt;",O23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11:R11">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="&lt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;",O11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U5">
+    <cfRule type="expression" priority="25">
+      <formula>E31=TRUE</formula>
+    </cfRule>
+    <cfRule type="expression" priority="26">
+      <formula>"E28=TRUE"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O26:R26">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&lt;">
-      <formula>NOT(ISERROR(SEARCH("&lt;",O11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("&lt;",O26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>